<commit_message>
script ipynb convertido para .py
</commit_message>
<xml_diff>
--- a/PesquisarPreço/arquivos/resultados/iphone.xlsx
+++ b/PesquisarPreço/arquivos/resultados/iphone.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +452,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -466,7 +466,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.enjoei.com.br/p/iphone-12-64gb-87683383%3Fg_campaign%3Dgoogle_shopping&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECOEM&amp;usg=AOvVaw0Jkel7-VFQUWRh08GstJ5U</t>
+          <t>https://www.google.com/url?url=https://www.enjoei.com.br/p/iphone-12-64gb-87683383%3Fg_campaign%3Dgoogle_shopping&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECKUM&amp;usg=AOvVaw0HEdaYZq-SYghYeEUP_w40</t>
         </is>
       </c>
     </row>
@@ -486,7 +486,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.casasbahia.com.br/usado-iphone-12-64gb-preto-bom-trocafone-1560060485/p/1560060485%3Futm_medium%3DCpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1560060485%26idLojista%3D88259%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECP0L&amp;usg=AOvVaw3h-f7sjmgq9-Bsa0L8Oefx</t>
+          <t>https://www.google.com/url?url=https://www.casasbahia.com.br/usado-iphone-12-64gb-preto-bom-trocafone-1560060485/p/1560060485%3Futm_medium%3DCpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1560060485%26idLojista%3D88259%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECNEL&amp;usg=AOvVaw3H4UEYnJ9x1JsqabT1uPAl</t>
         </is>
       </c>
     </row>
@@ -506,13 +506,13 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.buscape.com.br/lead%3Foid%3D982639946%26sortorder%3D-1%26index%3D%26searchterm%3Dnull%26pagesize%3D-1%26channel%3D%26pla%3D2023-07-17T15:07:56.318578&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECI4M&amp;usg=AOvVaw1TVef_CD9DL-_KalyJWAKH</t>
+          <t>https://www.google.com/url?url=https://www.buscape.com.br/lead%3Foid%3D982639946%26sortorder%3D-1%26index%3D%26searchterm%3Dnull%26pagesize%3D-1%26channel%3D%26pla%3D2023-07-17T18:27:01.613566&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECOIL&amp;usg=AOvVaw0W5BygtyF2cC4y8US1y31n</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -526,7 +526,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://doji.com.br/product/apple-iphone-12-product-red-64gb-muito-bom&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECKAR&amp;usg=AOvVaw11tG7OguOxuEu4StW1lHnG</t>
+          <t>https://www.google.com/url?url=https://doji.com.br/product/apple-iphone-12-product-red-64gb-muito-bom&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECJAQ&amp;usg=AOvVaw1DpkKKDQEWv6_30QTSnbJ1</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.magazineluiza.com.br/usado-iphone-12-64gb-azul-muito-bom-trocafone-apple/p/cg0240c21g/te/ceba%3F%26seller_id%3Dtrocafone&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECMoL&amp;usg=AOvVaw3W2TY36P5em8NHtXCdGXNN</t>
+          <t>https://www.google.com/url?url=https://www.magazineluiza.com.br/usado-iphone-12-64gb-azul-muito-bom-trocafone-apple/p/cg0240c21g/te/ceba%3F%26seller_id%3Dtrocafone&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECJ4L&amp;usg=AOvVaw1N_6QEgI4rLb6tpiFHgT66</t>
         </is>
       </c>
     </row>
@@ -566,13 +566,13 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.magazineluiza.com.br/usado-iphone-12-64gb-preto-excelente-trocafone-apple/p/bd2aggd0fb/te/ceba%3F%26seller_id%3Dtrocafone&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECJ8M&amp;usg=AOvVaw2Y7D6BCL1dmeHmn9wBo2Uv</t>
+          <t>https://www.google.com/url?url=https://www.magazineluiza.com.br/usado-iphone-12-64gb-preto-excelente-trocafone-apple/p/bd2aggd0fb/te/ceba%3F%26seller_id%3Dtrocafone&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECPML&amp;usg=AOvVaw1p5OqFgNN-ilTF3XfkiJxx</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -586,107 +586,107 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://produto.mercadolivre.com.br/MLB-3092859645-apple-iphone-12-64gb-5g-vitrine-original-com-garantia-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECPkN&amp;usg=AOvVaw00Q5prPAfavrk0dsV4eeAh</t>
+          <t>https://www.google.com/url?url=https://produto.mercadolivre.com.br/MLB-3092859645-apple-iphone-12-64gb-5g-vitrine-original-com-garantia-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECK0N&amp;usg=AOvVaw1qHABMIv9uFBH6QkEtB0_Q</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>iphone 12 64gb tela 6.1 sem carregador e fone apple - preto</t>
+          <t>(seminovo) iphone 12 apple azul, 64gb</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>R$ 3.198,00</t>
+          <t>R$ 3.199,00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.buscape.com.br/lead%3Foid%3D942845168%26sortorder%3D-1%26index%3D%26searchterm%3Dnull%26pagesize%3D-1%26channel%3D%26pla%3D2023-07-17T18:31:06.114165&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECIMN&amp;usg=AOvVaw0L6VAChtirm-TMXVU8pkdY</t>
+          <t>https://www.google.com/url?url=https://www.taqi.com.br/seminovo-apple-iphone-12-64gb-azul-internacional-taqi/222835%3Fsrsltid%3DASuE1wRi8iT3ZmfeZGqnH8OEvju7K5QKzBvfv75GERY3MKeec30Kn7cfAXg&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECPIQ&amp;usg=AOvVaw0R_DBH9t3uQJ9BBWI9LYK9</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>smartphone apple iphone 12 64gb câmera dupla</t>
+          <t>(seminovo) iphone 12 apple verde, 64gb</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>R$ 3.198,00</t>
+          <t>R$ 3.199,00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.buscape.com.br/celular/smartphone-apple-iphone-12-64gb-ios?_lc=88&amp;searchterm=iphone%2012%2064gb</t>
+          <t>https://www.google.com/url?url=https://www.taqi.com.br/seminovo-apple-iphone-12-64gb-verde-taqi/222821%3Fsrsltid%3DASuE1wRy4_JH3cptIQO2n-YBRmD9lU-x5KogQ4W0SHCWntiBlixk1hl3OZQ&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECKEQ&amp;usg=AOvVaw201igPj67JVPW3HDeF7GX1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>iphone 12 64gb tela 6.1 sem carregador e fone apple - branco</t>
+          <t>vitrine apple iphone 12 64gb original 10x sem juros + brinde</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>R$ 3.198,00</t>
+          <t>R$ 3.199,00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.buscape.com.br/lead%3Foid%3D707343148%26sortorder%3D-1%26index%3D%26searchterm%3Dnull%26pagesize%3D-1%26channel%3D%26pla%3D2023-07-17T18:25:58.031359&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECLAM&amp;usg=AOvVaw2fy5nIiO1Vbuee0wAdfXkW</t>
+          <t>https://www.google.com/url?url=https://produto.mercadolivre.com.br/MLB-3768478292-vitrine-apple-iphone-12-64gb-original-10x-sem-juros-brinde-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECJER&amp;usg=AOvVaw1OoWk9jZ4pxMfiatl9mzN6</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>vitrine apple iphone 12 64gb original 10x sem juros + brinde</t>
+          <t>vitrine iphone 12 verde 64gb</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>R$ 3.199,00</t>
+          <t>R$ 3.199,99</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://produto.mercadolivre.com.br/MLB-3768478292-vitrine-apple-iphone-12-64gb-original-10x-sem-juros-brinde-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECIAS&amp;usg=AOvVaw3vm8HaLxXNUpatZWIRkQ_b</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/vitrine-iphone-12-verde-64gb-mp931589150/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECIQM&amp;usg=AOvVaw2WDUcALl49DV0ASHTXZh-Y</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>(seminovo) iphone 12 apple azul, 64gb</t>
+          <t>usado: iphone 12 64gb preto excelente - trocafone</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>R$ 3.199,00</t>
+          <t>R$ 3.239,10</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.taqi.com.br/seminovo-apple-iphone-12-64gb-azul-internacional-taqi/222835%3Fsrsltid%3DASuE1wSqmhVNaetFWK_HssGaLO60RAvwNvlVNcXIT5_dAEXJYeNDPqN9C1I&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECNER&amp;usg=AOvVaw0hlbn1upjphr850GiLWZ4c</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/usado-iphone-12-64gb-preto-excelente-trocafone-mp928594174/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECPQR&amp;usg=AOvVaw0cW6Sba1Y-98uc1ZOXqUR9</t>
         </is>
       </c>
     </row>
@@ -696,457 +696,417 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>(seminovo) iphone 12 apple verde, 64gb</t>
+          <t>aparelho iphone 12 preto 64gb apple seminovo/vitrine sem riscos com acessorios</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>R$ 3.199,00</t>
+          <t>R$ 3.289,90</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.taqi.com.br/seminovo-apple-iphone-12-64gb-verde-taqi/222821%3Fsrsltid%3DASuE1wTHIwfeTlHSUQjeklO6w9lFxSeNWHwoHB2dcqpLe_H8-rbDuLUBKWY&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECPEQ&amp;usg=AOvVaw2JZd6B-BhIiDT0Kctncho9</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/aparelho-iphone-12-preto-64gb-apple-seminovovitrine-sem-riscos-com-acessorios-mp934027394/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECLEQ&amp;usg=AOvVaw0WsqZ_HzvAb-WJK1JTXh0n</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>vitrine iphone 12 verde 64gb</t>
+          <t>iphone 12 64gb usado varias cores + carregador</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>R$ 3.199,99</t>
+          <t>R$ 3.330,00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/vitrine-iphone-12-verde-64gb-mp931589150/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECMAM&amp;usg=AOvVaw1UrfE9zruOTw7mkvocC1G7</t>
+          <t>https://www.google.com/url?url=https://www.americanas.com.br/produto/7436674444/iphone-12-64gb-usado-varias-cores-carregador%3Fopn%3DYSMESP%26offerId%3D6494a19c579fbc8d91ddcc4c%26srsltid%3DASuE1wSvCVRZp5bpvi3Rk9eeypGd7wZYfu9-pmpvkQ6MEYEB_HYmGiih4vo&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQguUECPkM&amp;usg=AOvVaw2YEY6kxWbqKhBj1JCPTgd1</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>usado: iphone 12 64gb preto excelente - trocafone</t>
+          <t>celular apple iphone 12 branco 64gb seminovo/vitrine + fonte e cabo</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>R$ 3.239,10</t>
+          <t>R$ 3.334,90</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/usado-iphone-12-64gb-preto-excelente-trocafone-mp928594174/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECNMS&amp;usg=AOvVaw00TeKzOsZTiisbyhiwmQOb</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-apple-iphone-12-branco-64gb-seminovovitrine-fonte-e-cabo-mp934027359/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECLER&amp;usg=AOvVaw3NI6ngcG5t3x2eoTKgCPGS</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>aparelho iphone 12 preto 64gb apple seminovo/vitrine sem riscos com acessorios</t>
+          <t>aparelho iphone 12 preto 64gb apple vitrine/seminovo com acessórios</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>R$ 3.289,90</t>
+          <t>R$ 3.344,90</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/aparelho-iphone-12-preto-64gb-apple-seminovovitrine-sem-riscos-com-acessorios-mp934027394/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECM8Q&amp;usg=AOvVaw10MifVvvZORphxe1kA74Jv</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/aparelho-iphone-12-preto-64gb-apple-vitrineseminovo-com-acessorios-mp934027315/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECIIR&amp;usg=AOvVaw1vJHB-yfOX7ICfQZuqqTmi</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>iphone 12 64gb usado varias cores + carregador</t>
+          <t>iphone 12 64gb branco de vitrine tela 6,1&amp;quot; 4g câmera traseira 12mp+12mp ...</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>R$ 3.330,00</t>
+          <t>R$ 3.349,00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.americanas.com.br/produto/7436674444/iphone-12-64gb-usado-varias-cores-carregador%3Fopn%3DYSMESP%26offerId%3D6494a19c579fbc8d91ddcc4c%26srsltid%3DASuE1wRzcGyF7TkrLhygfqI1Lm7RPusOrr_-g25A78re-UpTeWgzW7MzD6o&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQguUECMUN&amp;usg=AOvVaw1avledI_HwxqxooMvQH57f</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/iphone-12-64gb-branco-de-vitrine-tela-61quot-4g-camera-traseira-12mp12mp-vitrine-mp932521352/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECOkM&amp;usg=AOvVaw3hpJIcRPeelbHMhjS6p7yO</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>celular apple iphone 12 branco 64gb seminovo/vitrine + fonte e cabo</t>
+          <t>iphone 12 64gb roxo tela 6,1 4g câmera traseira 12mp vitrine</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>R$ 3.334,90</t>
+          <t>R$ 3.349,00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-apple-iphone-12-branco-64gb-seminovovitrine-fonte-e-cabo-mp934027359/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECJAS&amp;usg=AOvVaw2lxVx6YxURW2xhW7crQlls</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/iphone-12-64gb-roxo-tela-61-4g-camera-traseira-12mp-vitrine-mp932882255/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQguUECMEL&amp;usg=AOvVaw15Ev5jpmJ6IiTWPz3lRTWx</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>aparelho iphone 12 preto 64gb apple vitrine/seminovo com acessórios</t>
+          <t>usado: iphone 12 64gb preto muito bom - trocafone</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>R$ 3.344,90</t>
+          <t>R$ 3.379,00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/aparelho-iphone-12-preto-64gb-apple-vitrineseminovo-com-acessorios-mp934027315/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECLER&amp;usg=AOvVaw2TmI3DN6K8mRYjijQEXV1k</t>
+          <t>https://www.google.com/url?url=https://www.colombo.com.br/produto/Smartphone-e-Celular/Usado-iPhone-12-64GB-Preto-Muito-Bom-Trocafone-Preto%3Fportal%3D8B36E9207C24C76E6719268E49201D94%26srsltid%3DASuE1wQcQTF49Lq-4e9LxigLAKf1YV8ZcswbQIsnEFlsp1AJrtl9QJMMVX0&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECM0N&amp;usg=AOvVaw1YsNDl_ue2u3kmjas3ekTd</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>iphone 12 64gb branco de vitrine tela 6,1&amp;quot; 4g câmera traseira 12mp+12mp ...</t>
+          <t>celular apple iphone 12 black 64gb vitrine/seminovo com carrregador e cabo</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>R$ 3.349,00</t>
+          <t>R$ 3.379,90</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/iphone-12-64gb-branco-de-vitrine-tela-61quot-4g-camera-traseira-12mp12mp-vitrine-mp932521352/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECLUN&amp;usg=AOvVaw0kLlEVs3R9oBjxMzKEQzB2</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-apple-iphone-12-black-64gb-vitrineseminovo-com-carrregador-e-cabo-mp934027523/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECJQM&amp;usg=AOvVaw3gLWb8ssRx2LYFGx6vUx8U</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>iphone 12 64gb roxo tela 6,1 4g câmera traseira 12mp vitrine</t>
+          <t>aparelho iphone 12 64gb white apple seminovo/vitrine + fone tws e pelicula hydrogel</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>R$ 3.349,00</t>
+          <t>R$ 3.394,90</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/iphone-12-64gb-roxo-tela-61-4g-camera-traseira-12mp-vitrine-mp932882255/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQguUECO0L&amp;usg=AOvVaw1z9-TOOD02jZHrVkGNi8VJ</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/aparelho-iphone-12-64gb-white-apple-seminovovitrine-fone-tws-e-pelicula-hydrogel-mp934027386/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECMQS&amp;usg=AOvVaw1Wmn8Q--6I-D9FVfyBmZXc</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>usado: iphone 12 64gb preto muito bom - trocafone</t>
+          <t>celular apple iphone 12 white 64gb vitrine/seminovo + acessorios</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>R$ 3.379,00</t>
+          <t>R$ 3.445,90</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.colombo.com.br/produto/Smartphone-e-Celular/Usado-iPhone-12-64GB-Preto-Muito-Bom-Trocafone-Preto%3Fportal%3D8B36E9207C24C76E6719268E49201D94%26srsltid%3DASuE1wSv1Z7JRmOkx_Jje2gDL4epJdhplO_DCY2lY-oxGc4E5yCnRAfyk0M&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECKsO&amp;usg=AOvVaw0NWAGX3Trv-r4DWHT1OTPm</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-apple-iphone-12-white-64gb-vitrineseminovo-acessorios-mp934027474/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECKEO&amp;usg=AOvVaw0SxgniQfMdp0W10M5eXoty</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>celular apple iphone 12 black 64gb vitrine/seminovo com carrregador e cabo</t>
+          <t>usado: iphone 12 64gb azul muito bom - trocafone</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>R$ 3.379,90</t>
+          <t>R$ 3.459,00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-apple-iphone-12-black-64gb-vitrineseminovo-com-carrregador-e-cabo-mp934027523/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECNAM&amp;usg=AOvVaw2ZDDNrqEKA4ryifIOcyPkQ</t>
+          <t>https://www.google.com/url?url=https://www.pontofrio.com.br/usado-iphone-12-64gb-azul-muito-bom-trocafone-1560061185/p/1560061185%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1560061185%26idLojista%3D88259%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECLYM&amp;usg=AOvVaw1ZbESAH4UAQ7bS5ghjOFng</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>celular apple iphone 12 white 64gb vitrine/seminovo + acessorios</t>
+          <t>celular iphone 12 white 64gb apple vitrine/seminovo com acessórios</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>R$ 3.445,90</t>
+          <t>R$ 3.494,90</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-apple-iphone-12-white-64gb-vitrineseminovo-acessorios-mp934027474/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECLwO&amp;usg=AOvVaw0drrGQ21Dw-ZbEbNEONpzL</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-iphone-12-white-64gb-apple-vitrineseminovo-com-acessorios-mp934027374/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECMIR&amp;usg=AOvVaw0ZRyBCIm6vUwafswhjJsjA</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>usado: iphone 12 64gb azul muito bom - trocafone</t>
+          <t>celular iphone 12 64gb black apple vitrine/seminovo com fonte e cabo</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>R$ 3.459,00</t>
+          <t>R$ 3.494,90</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.pontofrio.com.br/usado-iphone-12-64gb-azul-muito-bom-trocafone-1560061185/p/1560061185%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1560061185%26idLojista%3D88259%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECPIM&amp;usg=AOvVaw3-HbCHG6l25uB19ABiXXWk</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-iphone-12-64gb-black-apple-vitrineseminovo-com-fonte-e-cabo-mp934027339/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECNAP&amp;usg=AOvVaw2OqKwgdx_AYcaN2zRudnOy</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>celular iphone 12 white 64gb apple vitrine/seminovo com acessórios</t>
+          <t>iphone xr 64gb branco, com tela de 6,1, 4g, e câmera de 12 mp - mh6n3br/a</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>R$ 3.494,90</t>
+          <t>R$ 3.598,92</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-iphone-12-white-64gb-apple-vitrineseminovo-com-acessorios-mp934027374/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECKES&amp;usg=AOvVaw0ETVqJRlVpfIfurB3N9ADZ</t>
+          <t>https://www.google.com/url?url=https://www.vicvictor.com.br/XR-64-WHITE&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQguUECNgM&amp;usg=AOvVaw0w2jOmuyuPg1_5-g7wEI6A</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>celular iphone 12 64gb black apple vitrine/seminovo com fonte e cabo</t>
+          <t>celular iphone xr apple 64gb tela 6,1” 12mp</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>R$ 3.494,90</t>
+          <t>R$ 3.609,98</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-iphone-12-64gb-black-apple-vitrineseminovo-com-fonte-e-cabo-mp934027339/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECJ8P&amp;usg=AOvVaw1V0rzJaFWy0DYCCmNgfDo9</t>
+          <t>https://www.google.com/url?url=https://www.forcetech.com.br/products/iphone-xr-64gb%3Fvariant%3D39626988978327%26srsltid%3DASuE1wQZfDf8XUFWNWoyiwAB8lig9Aw4_Ea_DPrK_1sf7ODDxnxbPc_HibA&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECM8O&amp;usg=AOvVaw3JXSGT6RC9SEsxPGQC9AEP</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>iphone xr 64gb branco, com tela de 6,1, 4g, e câmera de 12 mp - mh6n3br/a</t>
+          <t>apple iphone 12 64gb semi novo - tela 6,1 5g câmera traseira 12mp ios - preto</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>R$ 3.598,92</t>
+          <t>R$ 3.679,00</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.vicvictor.com.br/XR-64-WHITE&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQguUECKQN&amp;usg=AOvVaw2P4HHou_w6RJpQTU66MmLW</t>
+          <t>https://www.google.com/url?url=https://www.hiperstorebrasil.com.br/produtos/apple-iphone-12-64gb-semi-novo-tela-61-5g-camera-traseira-12mp-ios-preto/&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECPEP&amp;usg=AOvVaw16-7Om_MYu8LJ47Pp2qQPX</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>celular iphone xr apple 64gb tela 6,1” 12mp</t>
+          <t>apple iphone 12 64gb semi novo - tela 6,1 5g câmera traseira 12mp ios - azul</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>R$ 3.609,98</t>
+          <t>R$ 3.679,00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.forcetech.com.br/products/iphone-xr-64gb%3Fvariant%3D39626988978327%26srsltid%3DASuE1wSLOywxsLs2ovHsH3fYnSwUXyrHdZE7yRB5Q3d59HCAAOrYqzb-Lzc&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECL4P&amp;usg=AOvVaw08Mv4WdttzjCsCsdyvEBh-</t>
+          <t>https://www.google.com/url?url=https://www.hiperstorebrasil.com.br/produtos/apple-iphone-12-64gb-semi-novo-tela-61-5g-camera-traseira-12mp-ios-azul/&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECLEP&amp;usg=AOvVaw3jeQCbh3oVnVvDwDT9xccZ</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>apple iphone 12 64gb semi novo - tela 6,1 5g câmera traseira 12mp ios - azul</t>
+          <t>aparelho iphone 12 64gb black apple com fone bluetooth e pelicula hydrogel ...</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>R$ 3.679,00</t>
+          <t>R$ 3.679,90</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.hiperstorebrasil.com.br/produtos/apple-iphone-12-64gb-semi-novo-tela-61-5g-camera-traseira-12mp-ios-azul/&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECKAQ&amp;usg=AOvVaw3K9DM-S6MEvwPIbrA8R5RT</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/aparelho-iphone-12-64gb-black-apple-com-fone-bluetooth-e-pelicula-hydrogel-vitrineseminovo-mp934027469/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECIUS&amp;usg=AOvVaw0GI_FbX6ZDOXwpflvs07_I</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>apple iphone 12 64gb semi novo - tela 6,1 5g câmera traseira 12mp ios - preto</t>
+          <t>apple iphone 12 64gb - 12mp ios - tela super retina xdr oled 6.1" - preto</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>R$ 3.679,00</t>
+          <t>R$ 3.694,55</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.hiperstorebrasil.com.br/produtos/apple-iphone-12-64gb-semi-novo-tela-61-5g-camera-traseira-12mp-ios-preto/&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECIER&amp;usg=AOvVaw1MVwbzynAQVlC0GUfCj5kl</t>
+          <t>https://www.google.com/url?url=https://www.horizonplay.com.br/apple/iphone/apple-iphone-12-64gb-azul-novo-lacrado-tela-super-retina-xdr-oled-6-1%3Fvariant_id%3D21019%26parceiro%3D8926%26srsltid%3DASuE1wRJMBCWeLc2TZ0g_B4Xihe5zkZucDJC7ojha1t0lRyQL43YUZcG39k&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECMcM&amp;usg=AOvVaw05blWue1DrvWxbAvvSGts5</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>aparelho iphone 12 64gb black apple com fone bluetooth e pelicula hydrogel ...</t>
+          <t>aparelho apple iphone 12 64gb preto vitrine/semi-novo com acessorios</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>R$ 3.679,90</t>
+          <t>R$ 3.699,00</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/aparelho-iphone-12-64gb-black-apple-com-fone-bluetooth-e-pelicula-hydrogel-vitrineseminovo-mp934027469/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECOQS&amp;usg=AOvVaw085kmO_UBLMs1b1qQZgFkA</t>
+          <t>https://www.google.com/url?url=https://www.riachuelo.com.br/produto/aparelho-apple-iphone-12-64gb-preto-vitrine-semi-novo-com-acessorios-3f1e30666e5f4694971d75ff2d76792c%3Fsku%3DIp-12-P-00&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECL0N&amp;usg=AOvVaw0otTJyRMRUKm_9nZXc4crI</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>apple iphone 12 64gb - 12mp ios - tela super retina xdr oled 6.1" - preto</t>
+          <t>iphone 12 apple vermelho, 64gb</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>R$ 3.694,55</t>
+          <t>R$ 3.699,00</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.horizonplay.com.br/apple/iphone/apple-iphone-12-64gb-azul-novo-lacrado-tela-super-retina-xdr-oled-6-1%3Fvariant_id%3D21019%26parceiro%3D8926%26srsltid%3DASuE1wSiWDEy_aZe9-8to-gZj0E15ervLAPmd-FpRfUvJIorwiMuqD5LuMc&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECJMN&amp;usg=AOvVaw2ttFAn09jqiCWGNrT8Dgtf</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>iphone 12 apple vermelho, 64gb</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>R$ 3.699,00</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>https://www.google.com/url?url=https://www.iplace.com.br/iphone-12-apple-vermelho-64gb-mgj73br-a/216222%3Fsrsltid%3DASuE1wR7YZGIzMl5BSLoDaSBiM2KSXNoeRiGTMsR2qW5gfm8olgUSw5JNLc&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQguUECLkL&amp;usg=AOvVaw2mN9ViGITstHuSiYNhpuzC</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>aparelho apple iphone 12 64gb preto vitrine/semi-novo com acessorios</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>R$ 3.699,00</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>https://www.google.com/url?url=https://www.riachuelo.com.br/produto/aparelho-apple-iphone-12-64gb-preto-vitrine-semi-novo-com-acessorios-3f1e30666e5f4694971d75ff2d76792c%3Fsku%3DIp-12-P-00&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiuwJ_16paAAxVwp5UCHexAAqAQgOUECIkO&amp;usg=AOvVaw0kbKbSJJZlG23tOWnZM88X</t>
+          <t>https://www.google.com/url?url=https://www.iplace.com.br/iphone-12-apple-vermelho-64gb-mgj73br-a/216222%3Fsrsltid%3DASuE1wS8IQ0nTPi6be2-8j2uue53-jXhjpKN_Sli6sWuzRTOx3IgFvYZiXw&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQguUECI0L&amp;usg=AOvVaw2MyOzmFrGI9XZaLCO3EjqF</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
implementação de janela para abrir e salvar aquivos
</commit_message>
<xml_diff>
--- a/PesquisarPreço/arquivos/resultados/iphone.xlsx
+++ b/PesquisarPreço/arquivos/resultados/iphone.xlsx
@@ -452,7 +452,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -466,7 +466,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.enjoei.com.br/p/iphone-12-64gb-87683383%3Fg_campaign%3Dgoogle_shopping&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECKUM&amp;usg=AOvVaw0HEdaYZq-SYghYeEUP_w40</t>
+          <t>https://www.google.com/url?url=https://www.enjoei.com.br/p/iphone-12-64gb-87683383%3Fg_campaign%3Dgoogle_shopping&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECLcM&amp;usg=AOvVaw1Z746G8DrIsUjdwIyA4Ma9</t>
         </is>
       </c>
     </row>
@@ -486,7 +486,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.casasbahia.com.br/usado-iphone-12-64gb-preto-bom-trocafone-1560060485/p/1560060485%3Futm_medium%3DCpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1560060485%26idLojista%3D88259%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECNEL&amp;usg=AOvVaw3H4UEYnJ9x1JsqabT1uPAl</t>
+          <t>https://www.google.com/url?url=https://www.casasbahia.com.br/usado-iphone-12-64gb-preto-bom-trocafone-1560060485/p/1560060485%3Futm_medium%3DCpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1560060485%26idLojista%3D88259%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECNIL&amp;usg=AOvVaw09Gcm2eXIapw58XGp2LpTR</t>
         </is>
       </c>
     </row>
@@ -506,13 +506,13 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.buscape.com.br/lead%3Foid%3D982639946%26sortorder%3D-1%26index%3D%26searchterm%3Dnull%26pagesize%3D-1%26channel%3D%26pla%3D2023-07-17T18:27:01.613566&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECOIL&amp;usg=AOvVaw0W5BygtyF2cC4y8US1y31n</t>
+          <t>https://www.google.com/url?url=https://www.buscape.com.br/lead%3Foid%3D982639946%26sortorder%3D-1%26index%3D%26searchterm%3Dnull%26pagesize%3D-1%26channel%3D%26pla%3D2023-07-17T18:27:01.613566&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECOML&amp;usg=AOvVaw34d7C02rFHkiX_PcSsumDN</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -526,13 +526,13 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://doji.com.br/product/apple-iphone-12-product-red-64gb-muito-bom&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECJAQ&amp;usg=AOvVaw1DpkKKDQEWv6_30QTSnbJ1</t>
+          <t>https://www.google.com/url?url=https://doji.com.br/product/apple-iphone-12-product-red-64gb-muito-bom&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECNEP&amp;usg=AOvVaw0j1si4lC1Z2HF9rjOFzefP</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -546,7 +546,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.magazineluiza.com.br/usado-iphone-12-64gb-azul-muito-bom-trocafone-apple/p/cg0240c21g/te/ceba%3F%26seller_id%3Dtrocafone&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECJ4L&amp;usg=AOvVaw1N_6QEgI4rLb6tpiFHgT66</t>
+          <t>https://www.google.com/url?url=https://www.magazineluiza.com.br/usado-iphone-12-64gb-azul-muito-bom-trocafone-apple/p/cg0240c21g/te/ceba%3F%26seller_id%3Dtrocafone&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECI0L&amp;usg=AOvVaw1CeHgeqM16HGm9xI1VlCsx</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.magazineluiza.com.br/usado-iphone-12-64gb-preto-excelente-trocafone-apple/p/bd2aggd0fb/te/ceba%3F%26seller_id%3Dtrocafone&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECPML&amp;usg=AOvVaw1p5OqFgNN-ilTF3XfkiJxx</t>
+          <t>https://www.google.com/url?url=https://www.magazineluiza.com.br/usado-iphone-12-64gb-preto-excelente-trocafone-apple/p/bd2aggd0fb/te/ceba%3F%26seller_id%3Dtrocafone&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECPQL&amp;usg=AOvVaw1IrH_NZxVPyygR0q5jIUnf</t>
         </is>
       </c>
     </row>
@@ -586,37 +586,37 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://produto.mercadolivre.com.br/MLB-3092859645-apple-iphone-12-64gb-5g-vitrine-original-com-garantia-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECK0N&amp;usg=AOvVaw1qHABMIv9uFBH6QkEtB0_Q</t>
+          <t>https://www.google.com/url?url=https://produto.mercadolivre.com.br/MLB-3092859645-apple-iphone-12-64gb-5g-vitrine-original-com-garantia-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECL8N&amp;usg=AOvVaw0gl3Q5gc7CyOJsG8bM-54K</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>(seminovo) iphone 12 apple azul, 64gb</t>
+          <t>smartphone apple iphone 12 64gb câmera dupla</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>R$ 3.199,00</t>
+          <t>R$ 3.198,00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.taqi.com.br/seminovo-apple-iphone-12-64gb-azul-internacional-taqi/222835%3Fsrsltid%3DASuE1wRi8iT3ZmfeZGqnH8OEvju7K5QKzBvfv75GERY3MKeec30Kn7cfAXg&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECPIQ&amp;usg=AOvVaw0R_DBH9t3uQJ9BBWI9LYK9</t>
+          <t>https://www.buscape.com.br/celular/smartphone-apple-iphone-12-64gb-ios?_lc=88&amp;searchterm=iphone%2012%2064gb</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>(seminovo) iphone 12 apple verde, 64gb</t>
+          <t>vitrine apple iphone 12 64gb original 10x sem juros + brinde</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -626,17 +626,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.taqi.com.br/seminovo-apple-iphone-12-64gb-verde-taqi/222821%3Fsrsltid%3DASuE1wRy4_JH3cptIQO2n-YBRmD9lU-x5KogQ4W0SHCWntiBlixk1hl3OZQ&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECKEQ&amp;usg=AOvVaw201igPj67JVPW3HDeF7GX1</t>
+          <t>https://www.google.com/url?url=https://produto.mercadolivre.com.br/MLB-3768478292-vitrine-apple-iphone-12-64gb-original-10x-sem-juros-brinde-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECPQR&amp;usg=AOvVaw0fe53gi4LsCSNQHDkrpkfS</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>vitrine apple iphone 12 64gb original 10x sem juros + brinde</t>
+          <t>(seminovo) iphone 12 apple azul, 64gb</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -646,107 +646,107 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://produto.mercadolivre.com.br/MLB-3768478292-vitrine-apple-iphone-12-64gb-original-10x-sem-juros-brinde-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECJER&amp;usg=AOvVaw1OoWk9jZ4pxMfiatl9mzN6</t>
+          <t>https://www.google.com/url?url=https://www.taqi.com.br/seminovo-iphone12-apple-azul64gb-nacional/220673%3Fsrsltid%3DASuE1wTNuRo9n6wt5uRqWfspiuyLoRgjnwScDy8JCXCJ6kVEIcNg81ocuoo&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECIMR&amp;usg=AOvVaw1f1gMZRTn2k6MUQP-LF9FD</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>vitrine iphone 12 verde 64gb</t>
+          <t>(seminovo) iphone 12 apple verde, 64gb</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>R$ 3.199,99</t>
+          <t>R$ 3.199,00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/vitrine-iphone-12-verde-64gb-mp931589150/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECIQM&amp;usg=AOvVaw2WDUcALl49DV0ASHTXZh-Y</t>
+          <t>https://www.google.com/url?url=https://www.taqi.com.br/seminovo-apple-iphone-12-64gb-verde-taqi/222821%3Fsrsltid%3DASuE1wQQzt1gQHFN8uiUtrP6HGGQF9-JXtHi-phshs3cPJAL5uqQFs_Khms&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECJMQ&amp;usg=AOvVaw2ekabuPf9rRcNhZqB_AKOI</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>usado: iphone 12 64gb preto excelente - trocafone</t>
+          <t>vitrine iphone 12 verde 64gb</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>R$ 3.239,10</t>
+          <t>R$ 3.199,99</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/usado-iphone-12-64gb-preto-excelente-trocafone-mp928594174/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECPQR&amp;usg=AOvVaw0cW6Sba1Y-98uc1ZOXqUR9</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/vitrine-iphone-12-verde-64gb-mp931589150/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECJYM&amp;usg=AOvVaw2zOMfBjHToudCAbVCE01ap</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>aparelho iphone 12 preto 64gb apple seminovo/vitrine sem riscos com acessorios</t>
+          <t>usado: iphone 12 64gb preto excelente - trocafone</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>R$ 3.289,90</t>
+          <t>R$ 3.239,10</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/aparelho-iphone-12-preto-64gb-apple-seminovovitrine-sem-riscos-com-acessorios-mp934027394/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECLEQ&amp;usg=AOvVaw0WsqZ_HzvAb-WJK1JTXh0n</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/usado-iphone-12-64gb-preto-excelente-trocafone-mp928594174/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECJQS&amp;usg=AOvVaw0jpC-av913KtusijqsLDxF</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>iphone 12 64gb usado varias cores + carregador</t>
+          <t>aparelho iphone 12 preto 64gb apple seminovo/vitrine sem riscos com acessorios</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>R$ 3.330,00</t>
+          <t>R$ 3.289,90</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.americanas.com.br/produto/7436674444/iphone-12-64gb-usado-varias-cores-carregador%3Fopn%3DYSMESP%26offerId%3D6494a19c579fbc8d91ddcc4c%26srsltid%3DASuE1wSvCVRZp5bpvi3Rk9eeypGd7wZYfu9-pmpvkQ6MEYEB_HYmGiih4vo&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQguUECPkM&amp;usg=AOvVaw2YEY6kxWbqKhBj1JCPTgd1</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/aparelho-iphone-12-preto-64gb-apple-seminovovitrine-sem-riscos-com-acessorios-mp934027394/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECOUR&amp;usg=AOvVaw0oxtgmeY0ITz08BCJly9tO</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>celular apple iphone 12 branco 64gb seminovo/vitrine + fonte e cabo</t>
+          <t>iphone 12 64gb usado varias cores + carregador</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>R$ 3.334,90</t>
+          <t>R$ 3.330,00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-apple-iphone-12-branco-64gb-seminovovitrine-fonte-e-cabo-mp934027359/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECLER&amp;usg=AOvVaw3NI6ngcG5t3x2eoTKgCPGS</t>
+          <t>https://www.google.com/url?url=https://www.americanas.com.br/produto/7436674444/iphone-12-64gb-usado-varias-cores-carregador%3Fopn%3DYSMESP%26offerId%3D6494a19c579fbc8d91ddcc4c%26srsltid%3DASuE1wQDcoDX_rFqjZJ5Kf_R5DFy7ye6NjNXRci_-bIHf8TULN1fAMuXoN4&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQguUECIsN&amp;usg=AOvVaw0qg5kb17uolvDPhP_9Ycbc</t>
         </is>
       </c>
     </row>
@@ -756,47 +756,47 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>aparelho iphone 12 preto 64gb apple vitrine/seminovo com acessórios</t>
+          <t>celular apple iphone 12 branco 64gb seminovo/vitrine + fonte e cabo</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>R$ 3.344,90</t>
+          <t>R$ 3.334,90</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/aparelho-iphone-12-preto-64gb-apple-vitrineseminovo-com-acessorios-mp934027315/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECIIR&amp;usg=AOvVaw1vJHB-yfOX7ICfQZuqqTmi</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-apple-iphone-12-branco-64gb-seminovovitrine-fonte-e-cabo-mp934027359/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECLIR&amp;usg=AOvVaw1RefdrUq-G5js2z6ZcuqXF</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>iphone 12 64gb branco de vitrine tela 6,1&amp;quot; 4g câmera traseira 12mp+12mp ...</t>
+          <t>aparelho iphone 12 preto 64gb apple vitrine/seminovo com acessórios</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>R$ 3.349,00</t>
+          <t>R$ 3.344,90</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/iphone-12-64gb-branco-de-vitrine-tela-61quot-4g-camera-traseira-12mp12mp-vitrine-mp932521352/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECOkM&amp;usg=AOvVaw3hpJIcRPeelbHMhjS6p7yO</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/aparelho-iphone-12-preto-64gb-apple-vitrineseminovo-com-acessorios-mp934027315/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECMMQ&amp;usg=AOvVaw3cwXpuki8hupMsALNqAQN4</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>iphone 12 64gb roxo tela 6,1 4g câmera traseira 12mp vitrine</t>
+          <t>iphone 12 64gb branco de vitrine tela 6,1&amp;quot; 4g câmera traseira 12mp+12mp ...</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -806,67 +806,67 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/iphone-12-64gb-roxo-tela-61-4g-camera-traseira-12mp-vitrine-mp932882255/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQguUECMEL&amp;usg=AOvVaw15Ev5jpmJ6IiTWPz3lRTWx</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/iphone-12-64gb-branco-de-vitrine-tela-61quot-4g-camera-traseira-12mp12mp-vitrine-mp932521352/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECOoM&amp;usg=AOvVaw2yK1CeEgKXaVdA_mngQlol</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>usado: iphone 12 64gb preto muito bom - trocafone</t>
+          <t>iphone 12 64gb roxo tela 6,1 4g câmera traseira 12mp vitrine</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>R$ 3.379,00</t>
+          <t>R$ 3.349,00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.colombo.com.br/produto/Smartphone-e-Celular/Usado-iPhone-12-64GB-Preto-Muito-Bom-Trocafone-Preto%3Fportal%3D8B36E9207C24C76E6719268E49201D94%26srsltid%3DASuE1wQcQTF49Lq-4e9LxigLAKf1YV8ZcswbQIsnEFlsp1AJrtl9QJMMVX0&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECM0N&amp;usg=AOvVaw1YsNDl_ue2u3kmjas3ekTd</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/iphone-12-64gb-roxo-tela-61-4g-camera-traseira-12mp-vitrine-mp932882255/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQguUECMIL&amp;usg=AOvVaw31OGzsIfTv2VMKirwGvfy_</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>celular apple iphone 12 black 64gb vitrine/seminovo com carrregador e cabo</t>
+          <t>usado: iphone 12 64gb preto muito bom - trocafone</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>R$ 3.379,90</t>
+          <t>R$ 3.379,00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-apple-iphone-12-black-64gb-vitrineseminovo-com-carrregador-e-cabo-mp934027523/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECJQM&amp;usg=AOvVaw3gLWb8ssRx2LYFGx6vUx8U</t>
+          <t>https://www.google.com/url?url=https://www.colombo.com.br/produto/Smartphone-e-Celular/Usado-iPhone-12-64GB-Preto-Muito-Bom-Trocafone-Preto%3Fportal%3D8B36E9207C24C76E6719268E49201D94%26srsltid%3DASuE1wST1EtotWOnnPSPgznqM4RsgdD3G5-sH5BgVBpO9NGiZKeqNxWji4s&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECN8N&amp;usg=AOvVaw0BRSeLywXWr9DNIO1oWE8K</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>aparelho iphone 12 64gb white apple seminovo/vitrine + fone tws e pelicula hydrogel</t>
+          <t>celular apple iphone 12 black 64gb vitrine/seminovo com carrregador e cabo</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>R$ 3.394,90</t>
+          <t>R$ 3.379,90</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/aparelho-iphone-12-64gb-white-apple-seminovovitrine-fone-tws-e-pelicula-hydrogel-mp934027386/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECMQS&amp;usg=AOvVaw1Wmn8Q--6I-D9FVfyBmZXc</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-apple-iphone-12-black-64gb-vitrineseminovo-com-carrregador-e-cabo-mp934027523/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECIUM&amp;usg=AOvVaw3dDC_yGYMulBzA0pLNeHYQ</t>
         </is>
       </c>
     </row>
@@ -886,13 +886,13 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-apple-iphone-12-white-64gb-vitrineseminovo-acessorios-mp934027474/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECKEO&amp;usg=AOvVaw0SxgniQfMdp0W10M5eXoty</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-apple-iphone-12-white-64gb-vitrineseminovo-acessorios-mp934027474/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECKMO&amp;usg=AOvVaw0zLDLhBdqkg0z9B7ZMgA67</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -906,13 +906,13 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.pontofrio.com.br/usado-iphone-12-64gb-azul-muito-bom-trocafone-1560061185/p/1560061185%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1560061185%26idLojista%3D88259%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECLYM&amp;usg=AOvVaw1ZbESAH4UAQ7bS5ghjOFng</t>
+          <t>https://www.google.com/url?url=https://www.pontofrio.com.br/usado-iphone-12-64gb-azul-muito-bom-trocafone-1560061185/p/1560061185%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1560061185%26idLojista%3D88259%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECKYM&amp;usg=AOvVaw3nZBQt01HtxSf5P5ydp_aB</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -926,13 +926,13 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-iphone-12-white-64gb-apple-vitrineseminovo-com-acessorios-mp934027374/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECMIR&amp;usg=AOvVaw0ZRyBCIm6vUwafswhjJsjA</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-iphone-12-white-64gb-apple-vitrineseminovo-com-acessorios-mp934027374/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECMMR&amp;usg=AOvVaw2Dbc8nu8DU6bCU59fkXxso</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -946,13 +946,13 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-iphone-12-64gb-black-apple-vitrineseminovo-com-fonte-e-cabo-mp934027339/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECNAP&amp;usg=AOvVaw2OqKwgdx_AYcaN2zRudnOy</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/celular-iphone-12-64gb-black-apple-vitrineseminovo-com-fonte-e-cabo-mp934027339/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECPIP&amp;usg=AOvVaw3PSQ0sL869-IWv0Sk7JhiS</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -966,7 +966,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.vicvictor.com.br/XR-64-WHITE&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQguUECNgM&amp;usg=AOvVaw0w2jOmuyuPg1_5-g7wEI6A</t>
+          <t>https://www.google.com/url?url=https://www.vicvictor.com.br/XR-64-WHITE&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQguUECMkM&amp;usg=AOvVaw0yv9PwtfWTFYzhFxqwC1jm</t>
         </is>
       </c>
     </row>
@@ -986,13 +986,13 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.forcetech.com.br/products/iphone-xr-64gb%3Fvariant%3D39626988978327%26srsltid%3DASuE1wQZfDf8XUFWNWoyiwAB8lig9Aw4_Ea_DPrK_1sf7ODDxnxbPc_HibA&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECM8O&amp;usg=AOvVaw3JXSGT6RC9SEsxPGQC9AEP</t>
+          <t>https://www.google.com/url?url=https://www.forcetech.com.br/products/iphone-xr-64gb%3Fvariant%3D39626988978327%26srsltid%3DASuE1wSIqQX-qOqVpLy0VI9EdkZFzs_8RvflS_IWpn8cLLUz4JvE7TieXrM&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECJMP&amp;usg=AOvVaw39OVi1P7z-_F1mm-pIYQO6</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1006,13 +1006,13 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.hiperstorebrasil.com.br/produtos/apple-iphone-12-64gb-semi-novo-tela-61-5g-camera-traseira-12mp-ios-preto/&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECPEP&amp;usg=AOvVaw16-7Om_MYu8LJ47Pp2qQPX</t>
+          <t>https://www.google.com/url?url=https://www.hiperstorebrasil.com.br/produtos/apple-iphone-12-64gb-semi-novo-tela-61-5g-camera-traseira-12mp-ios-preto/&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECKMQ&amp;usg=AOvVaw0Ipz6X6EhKLRwWEiwfOWwo</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.hiperstorebrasil.com.br/produtos/apple-iphone-12-64gb-semi-novo-tela-61-5g-camera-traseira-12mp-ios-azul/&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECLEP&amp;usg=AOvVaw3jeQCbh3oVnVvDwDT9xccZ</t>
+          <t>https://www.google.com/url?url=https://www.hiperstorebrasil.com.br/produtos/apple-iphone-12-64gb-semi-novo-tela-61-5g-camera-traseira-12mp-ios-azul/&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECOIP&amp;usg=AOvVaw0VvKddkvhwGy3UAMuPygjO</t>
         </is>
       </c>
     </row>
@@ -1046,13 +1046,13 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/aparelho-iphone-12-64gb-black-apple-com-fone-bluetooth-e-pelicula-hydrogel-vitrineseminovo-mp934027469/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECIUS&amp;usg=AOvVaw0GI_FbX6ZDOXwpflvs07_I</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/aparelho-iphone-12-64gb-black-apple-com-fone-bluetooth-e-pelicula-hydrogel-vitrineseminovo-mp934027469/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECLUS&amp;usg=AOvVaw2WyGD_GIKAuiuA4ThvJFlJ</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1066,17 +1066,17 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.horizonplay.com.br/apple/iphone/apple-iphone-12-64gb-azul-novo-lacrado-tela-super-retina-xdr-oled-6-1%3Fvariant_id%3D21019%26parceiro%3D8926%26srsltid%3DASuE1wRJMBCWeLc2TZ0g_B4Xihe5zkZucDJC7ojha1t0lRyQL43YUZcG39k&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECMcM&amp;usg=AOvVaw05blWue1DrvWxbAvvSGts5</t>
+          <t>https://www.google.com/url?url=https://www.horizonplay.com.br/apple/iphone/apple-iphone-12-64gb-azul-novo-lacrado-tela-super-retina-xdr-oled-6-1%3Fvariant_id%3D21019%26parceiro%3D8926%26srsltid%3DASuE1wTw6I48TMyK1G-OkLEl8B2W0yo4UVzIfrK9BQsXRS_N3humuZKkkh0&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECNoM&amp;usg=AOvVaw1ELm8PcvFSVQ7fOFmj6pV5</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>aparelho apple iphone 12 64gb preto vitrine/semi-novo com acessorios</t>
+          <t>iphone 12 apple vermelho, 64gb</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1086,17 +1086,17 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.riachuelo.com.br/produto/aparelho-apple-iphone-12-64gb-preto-vitrine-semi-novo-com-acessorios-3f1e30666e5f4694971d75ff2d76792c%3Fsku%3DIp-12-P-00&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQgOUECL0N&amp;usg=AOvVaw0otTJyRMRUKm_9nZXc4crI</t>
+          <t>https://www.google.com/url?url=https://www.iplace.com.br/iphone-12-apple-vermelho-64gb-mgj73br-a/216222%3Fsrsltid%3DASuE1wSOoIwnMxRXpS8Oz9yIVVQPmbx1wE0NmsEyhVKqpF7vg8uxrfMmJ_E&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQguUECJ8L&amp;usg=AOvVaw15epFm4vWNe9yTQvgKa_cs</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>iphone 12 apple vermelho, 64gb</t>
+          <t>aparelho apple iphone 12 64gb preto vitrine/semi-novo com acessorios</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.iplace.com.br/iphone-12-apple-vermelho-64gb-mgj73br-a/216222%3Fsrsltid%3DASuE1wS8IQ0nTPi6be2-8j2uue53-jXhjpKN_Sli6sWuzRTOx3IgFvYZiXw&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiC5db99ZaAAxU7qZUCHcE9DpgQguUECI0L&amp;usg=AOvVaw2MyOzmFrGI9XZaLCO3EjqF</t>
+          <t>https://www.google.com/url?url=https://www.riachuelo.com.br/produto/aparelho-apple-iphone-12-64gb-preto-vitrine-semi-novo-com-acessorios-3f1e30666e5f4694971d75ff2d76792c%3Fsku%3DIp-12-P-00&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiHzM7XgJeAAxXUqJUCHa3nA8UQgOUECM8N&amp;usg=AOvVaw3u_91_UsdL2OlK7T_wj_6N</t>
         </is>
       </c>
     </row>

</xml_diff>